<commit_message>
Simulation clean-up and cascaded controller implementation
Implemented a cascaded control using either rotational LQR or PID (using same values as on quad), using a position LQR controller.

Cleaned up code to use struct values.
</commit_message>
<xml_diff>
--- a/Quadrotor/develop/LQR Optimal K Conversion Table.xlsx
+++ b/Quadrotor/develop/LQR Optimal K Conversion Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_go\Desktop\Mesbahi Lab (RAIN)\Quadrotor Test Platform\Matlab Simulation\Quadrotor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_go\Documents\GitHub\Tom-Miesen\Quadrotor\develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D76E8EDE-84CA-4A50-A12E-4AFD1204EE0B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B9D0B4D3-5B78-4253-96C6-19BE3F2F16A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12648" windowHeight="6708" xr2:uid="{8D433FAF-745D-47DE-BE48-CE45D2CEB150}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A2" sqref="A2:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,154 +442,154 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>-7.4975292835646103E-3</v>
+        <v>-3.7207827015474401E-3</v>
       </c>
       <c r="B2">
-        <v>-7.4975292835639702E-3</v>
+        <v>3.7207827015459899E-3</v>
       </c>
       <c r="C2">
-        <v>0.48514992071526503</v>
+        <v>0.48514992071525398</v>
       </c>
       <c r="D2">
-        <v>-33.312494313692497</v>
+        <v>22.978005452784998</v>
       </c>
       <c r="E2">
-        <v>-33.312494313692</v>
+        <v>-22.9780054527942</v>
       </c>
       <c r="F2">
-        <v>0.67643245308414601</v>
+        <v>-14.1228776736695</v>
       </c>
       <c r="G2">
-        <v>-7.1436812340550304E-3</v>
+        <v>-4.1915215717182302E-3</v>
       </c>
       <c r="H2">
-        <v>-7.1436812340550399E-3</v>
+        <v>4.1915215717164096E-3</v>
       </c>
       <c r="I2">
-        <v>0.16335079127382701</v>
+        <v>0.16335079127382501</v>
       </c>
       <c r="J2">
-        <v>-8.0502414007930003</v>
+        <v>6.3675205592801101</v>
       </c>
       <c r="K2">
-        <v>-8.0502414007929897</v>
+        <v>-6.3675205592802602</v>
       </c>
       <c r="L2">
-        <v>1.5930776590190101</v>
+        <v>-3.8979899187855702</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>-7.49752928356422E-3</v>
+        <v>-3.7207827015493002E-3</v>
       </c>
       <c r="B3">
-        <v>7.4975292835649703E-3</v>
+        <v>-3.7207827015468399E-3</v>
       </c>
       <c r="C3">
-        <v>0.48514992071525598</v>
+        <v>0.48514992071525298</v>
       </c>
       <c r="D3">
-        <v>33.312494313693399</v>
+        <v>-22.978005452788299</v>
       </c>
       <c r="E3">
-        <v>-33.312494313693101</v>
+        <v>-22.978005452799199</v>
       </c>
       <c r="F3">
-        <v>-0.676432453084161</v>
+        <v>14.1228776736698</v>
       </c>
       <c r="G3">
-        <v>-7.1436812340548101E-3</v>
+        <v>-4.19152157171986E-3</v>
       </c>
       <c r="H3">
-        <v>7.1436812340555404E-3</v>
+        <v>-4.1915215717171104E-3</v>
       </c>
       <c r="I3">
-        <v>0.16335079127382801</v>
+        <v>0.16335079127382299</v>
       </c>
       <c r="J3">
-        <v>8.0502414007930199</v>
+        <v>-6.3675205592801598</v>
       </c>
       <c r="K3">
-        <v>-8.0502414007930092</v>
+        <v>-6.3675205592803303</v>
       </c>
       <c r="L3">
-        <v>-1.5930776590190101</v>
+        <v>3.8979899187855902</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>7.4975292835639399E-3</v>
+        <v>3.72078270154835E-3</v>
       </c>
       <c r="B4">
-        <v>-7.4975292835643501E-3</v>
+        <v>3.7207827015466898E-3</v>
       </c>
       <c r="C4">
-        <v>0.48514992071527202</v>
+        <v>0.48514992071524099</v>
       </c>
       <c r="D4">
-        <v>-33.312494313691403</v>
+        <v>22.978005452787801</v>
       </c>
       <c r="E4">
-        <v>33.312494313692703</v>
+        <v>22.978005452796399</v>
       </c>
       <c r="F4">
-        <v>-0.67643245308425204</v>
+        <v>14.1228776736697</v>
       </c>
       <c r="G4">
-        <v>7.1436812340545898E-3</v>
+        <v>4.1915215717190498E-3</v>
       </c>
       <c r="H4">
-        <v>-7.1436812340550503E-3</v>
+        <v>4.1915215717170402E-3</v>
       </c>
       <c r="I4">
-        <v>0.16335079127382601</v>
+        <v>0.16335079127382099</v>
       </c>
       <c r="J4">
-        <v>-8.0502414007930003</v>
+        <v>6.3675205592801296</v>
       </c>
       <c r="K4">
-        <v>8.0502414007930003</v>
+        <v>6.3675205592802904</v>
       </c>
       <c r="L4">
-        <v>-1.5930776590190101</v>
+        <v>3.89798991878552</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>7.4975292835647699E-3</v>
+        <v>3.7207827015473599E-3</v>
       </c>
       <c r="B5">
-        <v>7.4975292835649703E-3</v>
+        <v>-3.7207827015454898E-3</v>
       </c>
       <c r="C5">
-        <v>0.48514992071527202</v>
+        <v>0.48514992071524998</v>
       </c>
       <c r="D5">
-        <v>33.3124943136947</v>
+        <v>-22.978005452783901</v>
       </c>
       <c r="E5">
-        <v>33.312494313693598</v>
+        <v>22.978005452794601</v>
       </c>
       <c r="F5">
-        <v>0.67643245308423094</v>
+        <v>-14.1228776736702</v>
       </c>
       <c r="G5">
-        <v>7.1436812340551596E-3</v>
+        <v>4.1915215717182302E-3</v>
       </c>
       <c r="H5">
-        <v>7.1436812340557798E-3</v>
+        <v>-4.1915215717160401E-3</v>
       </c>
       <c r="I5">
-        <v>0.16335079127383101</v>
+        <v>0.16335079127382099</v>
       </c>
       <c r="J5">
-        <v>8.0502414007930305</v>
+        <v>-6.3675205592800701</v>
       </c>
       <c r="K5">
-        <v>8.0502414007930092</v>
+        <v>6.3675205592802602</v>
       </c>
       <c r="L5">
-        <v>1.5930776590190301</v>
+        <v>-3.8979899187855498</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -609,15 +609,15 @@
       </c>
       <c r="D8">
         <f>D2*PI()/180</f>
-        <v>-0.58141270782582277</v>
+        <v>0.40104185069230863</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:F8" si="0">E2*PI()/180</f>
-        <v>-0.58141270782581411</v>
+        <v>-0.40104185069246923</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>1.1805973473660419E-2</v>
+        <v>-0.24649071526193006</v>
       </c>
       <c r="G8">
         <v>-7.1436812340550304E-3</v>
@@ -630,15 +630,15 @@
       </c>
       <c r="J8">
         <f>J2*PI()/180</f>
-        <v>-0.1405032180241983</v>
+        <v>0.11113419894786869</v>
       </c>
       <c r="K8">
         <f>K2*PI()/180</f>
-        <v>-0.14050321802419813</v>
+        <v>-0.11113419894787131</v>
       </c>
       <c r="L8">
         <f>L2*PI()/180</f>
-        <v>2.7804450389845265E-2</v>
+        <v>-6.8032758292354556E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -653,15 +653,15 @@
       </c>
       <c r="D9">
         <f t="shared" ref="D9:F9" si="1">D3*PI()/180</f>
-        <v>0.58141270782583854</v>
+        <v>-0.40104185069236625</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>-0.58141270782583332</v>
+        <v>-0.40104185069255649</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>-1.1805973473660681E-2</v>
+        <v>0.24649071526193531</v>
       </c>
       <c r="G9">
         <v>-7.1436812340548101E-3</v>
@@ -674,15 +674,15 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9" si="2">J3*PI()/180</f>
-        <v>0.14050321802419866</v>
+        <v>-0.11113419894786956</v>
       </c>
       <c r="K9">
         <f t="shared" ref="K9:L11" si="3">K3*PI()/180</f>
-        <v>-0.14050321802419846</v>
+        <v>-0.11113419894787253</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
-        <v>-2.7804450389845265E-2</v>
+        <v>6.8032758292354917E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -697,15 +697,15 @@
       </c>
       <c r="D10">
         <f t="shared" ref="D10:F10" si="4">D4*PI()/180</f>
-        <v>-0.58141270782580368</v>
+        <v>0.40104185069235759</v>
       </c>
       <c r="E10">
         <f t="shared" si="4"/>
-        <v>0.58141270782582644</v>
+        <v>0.4010418506925077</v>
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>-1.180597347366227E-2</v>
+        <v>0.24649071526193356</v>
       </c>
       <c r="G10">
         <v>7.1436812340545898E-3</v>
@@ -718,15 +718,15 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10" si="5">J4*PI()/180</f>
-        <v>-0.1405032180241983</v>
+        <v>0.11113419894786902</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>0.1405032180241983</v>
+        <v>0.11113419894787185</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
-        <v>-2.7804450389845265E-2</v>
+        <v>6.8032758292353696E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -741,15 +741,15 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11:F11" si="6">D5*PI()/180</f>
-        <v>0.58141270782586119</v>
+        <v>-0.40104185069228954</v>
       </c>
       <c r="E11">
         <f t="shared" si="6"/>
-        <v>0.58141270782584209</v>
+        <v>0.40104185069247628</v>
       </c>
       <c r="F11">
         <f t="shared" si="6"/>
-        <v>1.1805973473661902E-2</v>
+        <v>-0.24649071526194224</v>
       </c>
       <c r="G11">
         <v>7.1436812340551596E-3</v>
@@ -762,15 +762,15 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11" si="7">J5*PI()/180</f>
-        <v>0.14050321802419882</v>
+        <v>-0.111134198947868</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>0.14050321802419846</v>
+        <v>0.11113419894787131</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>2.7804450389845616E-2</v>
+        <v>-6.8032758292354209E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>